<commit_message>
cleared out a bug
</commit_message>
<xml_diff>
--- a/data/Data_3.xlsx
+++ b/data/Data_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strathmoreuni-my.sharepoint.com/personal/john_muinde_o365_strathmore_edu/Documents/Documents/excel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{E19FE65A-D049-4768-9DDB-52A628699CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02416C68-A6AE-49C0-8298-C1CC5B4A1FA3}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{E19FE65A-D049-4768-9DDB-52A628699CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDC8F1E6-AB86-486A-B61E-1CA80267789C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="615" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATHIRIVER" sheetId="3" r:id="rId1"/>
@@ -3836,6 +3836,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4162,8 +4166,8 @@
   </sheetPr>
   <dimension ref="A1:R136"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4173,7 +4177,7 @@
     <col min="3" max="3" width="20" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="59" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" style="59" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" style="59" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.44140625" style="59" bestFit="1" customWidth="1"/>
@@ -8387,8 +8391,8 @@
   </sheetPr>
   <dimension ref="A1:S127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11105,8 +11109,8 @@
   </sheetPr>
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>